<commit_message>
server & work update
</commit_message>
<xml_diff>
--- a/Arbeitspakete.xlsx
+++ b/Arbeitspakete.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="38">
   <si>
     <t>Status</t>
   </si>
@@ -134,13 +134,7 @@
     <t>Probleme mit xstart(mit welchem user meldet sich der socket server? Ist xstart activ?)</t>
   </si>
   <si>
-    <t>Problem mit leistung und Blop, lieber verlinkungen.....</t>
-  </si>
-  <si>
     <t>beim öffnen der Tür -&gt; Eintrag in der Datenbank</t>
-  </si>
-  <si>
-    <t>Ermitteln wer hat die Tür aufgemacht... Eintrag in datenbank nur name der Datei, mittels socket user_id, etc</t>
   </si>
 </sst>
 </file>
@@ -281,8 +275,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="31">
+  <cellStyleXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -332,7 +328,7 @@
     <xf numFmtId="0" fontId="4" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="31">
+  <cellStyles count="33">
     <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
@@ -348,6 +344,7 @@
     <cellStyle name="Besuchter Link" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
@@ -363,6 +360,7 @@
     <cellStyle name="Link" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -695,7 +693,7 @@
   <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -758,21 +756,17 @@
       <c r="C8" t="s">
         <v>7</v>
       </c>
-      <c r="H8" s="15" t="s">
+      <c r="H8" s="15"/>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="2"/>
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="A9" s="5"/>
-      <c r="B9" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" t="s">
-        <v>38</v>
-      </c>
-      <c r="H9" s="15" t="s">
-        <v>39</v>
-      </c>
+      <c r="H9" s="15"/>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="4"/>

</xml_diff>